<commit_message>
Documentos de Verificación de Base de Datos e Inventario. Correcciones
</commit_message>
<xml_diff>
--- a/Desarrollo/Proyecto SuperShop/Manuales/Gestión/Cronograma del proyecto - G6.xlsx
+++ b/Desarrollo/Proyecto SuperShop/Manuales/Gestión/Cronograma del proyecto - G6.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="152">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>SS-PC.DOCX</t>
+  </si>
+  <si>
+    <t>Artadi G./Líder del proyecto, Caballero O., Canales G., Santa Cruz E., Ortiz A.</t>
   </si>
   <si>
     <t>S2</t>
@@ -165,9 +168,6 @@
     <t>SS-MOD.DOCX</t>
   </si>
   <si>
-    <t>Marcos Vásquez E./FE(FrontEnd)</t>
-  </si>
-  <si>
     <t>Especificar Requisito del Software 5:</t>
   </si>
   <si>
@@ -201,7 +201,7 @@
     <t>Documento de Arquitectura del Software</t>
   </si>
   <si>
-    <t>SS-DAI.DOCX</t>
+    <t>SS-DAS.DOCX</t>
   </si>
   <si>
     <t>Caballero Meza O./AD(Data Analist), Rojas P. (AR/QA)</t>
@@ -213,10 +213,10 @@
     <t>Documento de Diseño del Sistema de Inventario</t>
   </si>
   <si>
-    <t>SS-DEUI.PDF</t>
-  </si>
-  <si>
-    <t>Santa Cruz E./FE (FrontEnd), Marcos Vásquez E. (FE)</t>
+    <t>SS-DDSI.PDF</t>
+  </si>
+  <si>
+    <t>Santa Cruz E./FE (FrontEnd)</t>
   </si>
   <si>
     <t>S3 -S4</t>
@@ -228,7 +228,7 @@
     <t>Documento de Interfaz utilizada en el Sistema de Inventario.</t>
   </si>
   <si>
-    <t>SS-GE.PDF</t>
+    <t>SS-DISI.PDF</t>
   </si>
   <si>
     <t xml:space="preserve">Diseñar la base de datos </t>
@@ -255,81 +255,90 @@
     <t>SS-RDS.DOCX</t>
   </si>
   <si>
+    <t>Ortiz A. (BE)</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Realizar Sprint Retrospective</t>
+  </si>
+  <si>
+    <t>Reporte del Primer Sprint</t>
+  </si>
+  <si>
+    <t>SS-RPS.DOCX</t>
+  </si>
+  <si>
+    <t>Artadi G./Líder del proyecto, Caballero O., Canales G., Santa Cruz E., Ortiz A., Rojas. P</t>
+  </si>
+  <si>
+    <t>Hito 1 - Fin del Sprint #1</t>
+  </si>
+  <si>
+    <t>CODIFICACIÓN Y PRUEBAS</t>
+  </si>
+  <si>
+    <t>Añadir más requisitos de Software por el cliente</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requisitos</t>
+  </si>
+  <si>
+    <t>SS-DER.DOCX</t>
+  </si>
+  <si>
+    <t>Caballero Meza O./AD(Data Analist)</t>
+  </si>
+  <si>
+    <t>S5 - S6</t>
+  </si>
+  <si>
+    <t>Verificar y Actualizar el diseño del Sistema de Inventario</t>
+  </si>
+  <si>
+    <t>Documento de Verificación del Sistema de Inventario.</t>
+  </si>
+  <si>
+    <t>SS-DVSI.PDF</t>
+  </si>
+  <si>
+    <t>Verificar y Actualizar documento de Base de Datos</t>
+  </si>
+  <si>
+    <t>Documento de Verificación de la Base de Datos.</t>
+  </si>
+  <si>
+    <t>SS-DVBD.DOCX</t>
+  </si>
+  <si>
+    <t>Ortiz A. (BE), Caballero Meza O./DBA(Database Administrator)</t>
+  </si>
+  <si>
+    <t>Realizar el testeo de diversas funciones del software</t>
+  </si>
+  <si>
+    <t>Documento de Testeo de Funciones</t>
+  </si>
+  <si>
+    <t>SS-TEF.DOCX</t>
+  </si>
+  <si>
+    <t>Canales Borda G. (T), Santa Cruz E. (T), Rojas. P(QA)</t>
+  </si>
+  <si>
+    <t>Someter a pruebas unitarias el software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documento de Pruebas Unitarios </t>
+  </si>
+  <si>
+    <t>SS-PU.DOCX</t>
+  </si>
+  <si>
     <t>Ortiz A. (BE), Marcos Vásquez E. (FE)</t>
   </si>
   <si>
-    <t>S5</t>
-  </si>
-  <si>
-    <t>Realizar Sprint Retrospective</t>
-  </si>
-  <si>
-    <t>Reporte del Primer Sprint</t>
-  </si>
-  <si>
-    <t>SS-RPS.DOCX</t>
-  </si>
-  <si>
-    <t>Artadi G./Líder del proyecto, Caballero O., Canales G., Santa Cruz E., Ortiz A., Marcos E., Rojas. P</t>
-  </si>
-  <si>
-    <t>Hito 1 - Fin del Sprint #1</t>
-  </si>
-  <si>
-    <t>CODIFICACIÓN Y PRUEBAS</t>
-  </si>
-  <si>
-    <t>Añadir más requisitos de Software por el cliente</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requisitos</t>
-  </si>
-  <si>
-    <t>SS-DER.DOCX</t>
-  </si>
-  <si>
-    <t>Caballero Meza O./AD(Data Analist)</t>
-  </si>
-  <si>
-    <t>S5 - S6</t>
-  </si>
-  <si>
-    <t>Verificar y Actualizar el diseño del Sistema de Inventario</t>
-  </si>
-  <si>
-    <t>Documento de Verificación del Sistema de Inventario.</t>
-  </si>
-  <si>
-    <t>Verificar y Actualizar documento de Base de Datos</t>
-  </si>
-  <si>
-    <t>Documento de Verificación de la Base de Datos.</t>
-  </si>
-  <si>
-    <t>Ortiz A. (BE), Caballero Meza O./DBA(Database Administrator)</t>
-  </si>
-  <si>
-    <t>Realizar el testeo de diversas funciones del software</t>
-  </si>
-  <si>
-    <t>Documento de Testeo de Funciones</t>
-  </si>
-  <si>
-    <t>SS-TEF.DOCX</t>
-  </si>
-  <si>
-    <t>Canales Borda G. (T), Santa Cruz E. (T), Rojas. P(QA)</t>
-  </si>
-  <si>
-    <t>Someter a pruebas unitarias el software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documento de Pruebas Unitarios </t>
-  </si>
-  <si>
-    <t>SS-PU.DOCX</t>
-  </si>
-  <si>
     <t>S7</t>
   </si>
   <si>
@@ -354,16 +363,10 @@
     <t>Verificar y finalizar documento del diseño del Sistema de Inventario</t>
   </si>
   <si>
-    <t>Santa Cruz E. (T), Marcos Vásquez E. (FE)</t>
-  </si>
-  <si>
     <t>Verificar y finalizar documento de la Base de Datos</t>
   </si>
   <si>
     <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
-  </si>
-  <si>
-    <t>SS-DAS.DOCX</t>
   </si>
   <si>
     <t>Realizar Pruebas finales del Software</t>
@@ -476,7 +479,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -587,6 +590,13 @@
     </font>
     <font>
       <b/>
+      <i/>
+      <sz val="10.0"/>
+      <color rgb="FF060606"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
@@ -677,14 +687,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAEE7E8"/>
-        <bgColor rgb="FFAEE7E8"/>
+        <fgColor rgb="FF666666"/>
+        <bgColor rgb="FF666666"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFAFDCB"/>
-        <bgColor rgb="FFFAFDCB"/>
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1013,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1130,93 +1140,94 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="13" fillId="4" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="2" fontId="19" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="2" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="4" fontId="19" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="19" fillId="2" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="2" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="2" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="2" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="15" fillId="2" fontId="19" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="15" fillId="2" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="3" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="3" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="20" fillId="4" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="20" fillId="4" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="13" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="21" fillId="4" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="21" fillId="4" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="22" fillId="3" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="3" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="13" fillId="2" fontId="24" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="2" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="2" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="2" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="2" fontId="25" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="2" fontId="26" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="15" fillId="2" fontId="25" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="15" fillId="2" fontId="26" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="3" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="3" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="22" fillId="3" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="23" fillId="4" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="24" fillId="2" fontId="19" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="2" fontId="19" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="2" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="25" fillId="2" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="25" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="26" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="26" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="25" fillId="2" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="25" fillId="2" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="27" fillId="2" fontId="25" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="27" fillId="2" fontId="26" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="7" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="7" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1656,7 +1667,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F13" s="26">
         <v>45027.0</v>
@@ -1665,10 +1676,10 @@
         <v>45036.0</v>
       </c>
       <c r="H13" s="27">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J13" s="31"/>
       <c r="K13" s="5"/>
@@ -1676,16 +1687,16 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="29"/>
       <c r="B14" s="22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
@@ -1695,10 +1706,10 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="29"/>
       <c r="B15" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>18</v>
@@ -1720,16 +1731,16 @@
     <row r="16" ht="29.25" customHeight="1">
       <c r="A16" s="29"/>
       <c r="B16" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F16" s="26">
         <v>45027.0</v>
@@ -1746,16 +1757,16 @@
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="29"/>
       <c r="B17" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F17" s="26">
         <v>45021.0</v>
@@ -1763,8 +1774,8 @@
       <c r="G17" s="26">
         <v>45037.0</v>
       </c>
-      <c r="H17" s="27">
-        <v>0.0</v>
+      <c r="H17" s="40">
+        <v>1.0</v>
       </c>
       <c r="J17" s="31"/>
       <c r="K17" s="5"/>
@@ -1772,16 +1783,16 @@
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="29"/>
       <c r="B18" s="37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F18" s="26">
         <v>45021.0</v>
@@ -1790,7 +1801,7 @@
         <v>45046.0</v>
       </c>
       <c r="H18" s="40">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I18" s="28"/>
       <c r="J18" s="31"/>
@@ -1799,16 +1810,16 @@
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="29"/>
       <c r="B19" s="37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F19" s="26">
         <v>45021.0</v>
@@ -1826,16 +1837,16 @@
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="29"/>
       <c r="B20" s="37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F20" s="26">
         <v>45021.0</v>
@@ -1870,8 +1881,8 @@
       <c r="G21" s="26">
         <v>45042.0</v>
       </c>
-      <c r="H21" s="40">
-        <v>0.0</v>
+      <c r="H21" s="27">
+        <v>1.0</v>
       </c>
       <c r="I21" s="28"/>
       <c r="J21" s="31"/>
@@ -1926,8 +1937,8 @@
       <c r="G23" s="26">
         <v>45044.0</v>
       </c>
-      <c r="H23" s="40">
-        <v>0.0</v>
+      <c r="H23" s="27">
+        <v>1.0</v>
       </c>
       <c r="I23" s="28"/>
       <c r="J23" s="31"/>
@@ -1941,7 +1952,7 @@
       <c r="C24" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="39" t="s">
         <v>66</v>
       </c>
       <c r="E24" s="33" t="s">
@@ -1953,8 +1964,8 @@
       <c r="G24" s="26">
         <v>45044.0</v>
       </c>
-      <c r="H24" s="27">
-        <v>0.0</v>
+      <c r="H24" s="40">
+        <v>1.0</v>
       </c>
       <c r="I24" s="28" t="s">
         <v>68</v>
@@ -1970,7 +1981,7 @@
       <c r="C25" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="39" t="s">
         <v>71</v>
       </c>
       <c r="E25" s="33" t="s">
@@ -1982,8 +1993,8 @@
       <c r="G25" s="26">
         <v>45044.0</v>
       </c>
-      <c r="H25" s="27">
-        <v>0.0</v>
+      <c r="H25" s="40">
+        <v>1.0</v>
       </c>
       <c r="J25" s="31"/>
       <c r="K25" s="5"/>
@@ -2009,7 +2020,7 @@
         <v>45044.0</v>
       </c>
       <c r="H26" s="27">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J26" s="31"/>
       <c r="K26" s="5"/>
@@ -2019,7 +2030,7 @@
       <c r="B27" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="48"/>
       <c r="D27" s="24"/>
       <c r="E27" s="33"/>
       <c r="F27" s="26">
@@ -2052,7 +2063,7 @@
         <v>45046.0</v>
       </c>
       <c r="H28" s="27">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I28" s="28" t="s">
         <v>81</v>
@@ -2081,32 +2092,32 @@
         <v>45046.0</v>
       </c>
       <c r="H29" s="27">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J29" s="31"/>
       <c r="K29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="14"/>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="51">
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="52">
         <v>45027.0</v>
       </c>
-      <c r="G30" s="51">
+      <c r="G30" s="52">
         <v>45046.0</v>
       </c>
-      <c r="H30" s="52"/>
+      <c r="H30" s="53"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="54" t="s">
         <v>88</v>
       </c>
       <c r="C31" s="36" t="s">
@@ -2124,25 +2135,25 @@
       <c r="G31" s="26">
         <v>45054.0</v>
       </c>
-      <c r="H31" s="54">
+      <c r="H31" s="55">
         <v>0.0</v>
       </c>
       <c r="I31" s="28" t="s">
         <v>92</v>
       </c>
       <c r="J31" s="31"/>
-      <c r="K31" s="55"/>
+      <c r="K31" s="56"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="29"/>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="24" t="s">
-        <v>66</v>
+      <c r="D32" s="39" t="s">
+        <v>95</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>80</v>
@@ -2153,7 +2164,7 @@
       <c r="G32" s="26">
         <v>45054.0</v>
       </c>
-      <c r="H32" s="57">
+      <c r="H32" s="58">
         <v>0.0</v>
       </c>
       <c r="J32" s="31"/>
@@ -2161,17 +2172,17 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="29"/>
-      <c r="B33" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="56" t="s">
+      <c r="B33" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="24" t="s">
-        <v>74</v>
+      <c r="C33" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>98</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F33" s="26">
         <v>45047.0</v>
@@ -2179,7 +2190,7 @@
       <c r="G33" s="26">
         <v>45054.0</v>
       </c>
-      <c r="H33" s="54">
+      <c r="H33" s="55">
         <v>0.0</v>
       </c>
       <c r="J33" s="31"/>
@@ -2188,16 +2199,16 @@
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="29"/>
       <c r="B34" s="37" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F34" s="26">
         <v>45054.0</v>
@@ -2205,7 +2216,7 @@
       <c r="G34" s="26">
         <v>45054.0</v>
       </c>
-      <c r="H34" s="57">
+      <c r="H34" s="58">
         <v>0.0</v>
       </c>
       <c r="J34" s="31"/>
@@ -2214,16 +2225,16 @@
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="29"/>
       <c r="B35" s="37" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C35" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="33" t="s">
         <v>103</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="33" t="s">
-        <v>101</v>
       </c>
       <c r="F35" s="26">
         <v>45054.0</v>
@@ -2249,7 +2260,7 @@
         <v>79</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="F36" s="26">
         <v>45054.0</v>
@@ -2261,7 +2272,7 @@
         <v>0.0</v>
       </c>
       <c r="I36" s="28" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="J36" s="31"/>
       <c r="K36" s="5"/>
@@ -2272,10 +2283,10 @@
         <v>82</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E37" s="33" t="s">
         <v>85</v>
@@ -2294,28 +2305,28 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="61">
+        <v>111</v>
+      </c>
+      <c r="B38" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="60"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="62">
         <v>45047.0</v>
       </c>
-      <c r="G38" s="61">
+      <c r="G38" s="62">
         <v>45063.0</v>
       </c>
-      <c r="H38" s="62"/>
+      <c r="H38" s="63"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" s="63" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="B39" s="64" t="s">
+        <v>114</v>
       </c>
       <c r="C39" s="36" t="s">
         <v>89</v>
@@ -2341,17 +2352,17 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="29"/>
-      <c r="B40" s="53" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="56" t="s">
+      <c r="B40" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="24" t="s">
-        <v>66</v>
+      <c r="D40" s="39" t="s">
+        <v>95</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="F40" s="26">
         <v>45064.0</v>
@@ -2363,21 +2374,21 @@
         <v>0.0</v>
       </c>
       <c r="J40" s="31"/>
-      <c r="K40" s="64"/>
+      <c r="K40" s="65"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="29"/>
-      <c r="B41" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" s="24" t="s">
-        <v>74</v>
+      <c r="B41" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>98</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F41" s="26">
         <v>45064.0</v>
@@ -2394,13 +2405,13 @@
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="29"/>
       <c r="B42" s="22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>61</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="E42" s="33" t="s">
         <v>63</v>
@@ -2420,16 +2431,16 @@
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="29"/>
       <c r="B43" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F43" s="26">
         <v>45086.0</v>
@@ -2441,7 +2452,7 @@
         <v>0.0</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J43" s="31"/>
       <c r="K43" s="5"/>
@@ -2478,10 +2489,10 @@
         <v>82</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E45" s="33" t="s">
         <v>85</v>
@@ -2496,7 +2507,7 @@
         <v>0.0</v>
       </c>
       <c r="I45" s="28" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J45" s="31"/>
       <c r="K45" s="5"/>
@@ -2504,13 +2515,13 @@
     <row r="46" ht="25.5" customHeight="1">
       <c r="A46" s="29"/>
       <c r="B46" s="22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C46" s="36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E46" s="33" t="s">
         <v>85</v>
@@ -2529,17 +2540,17 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="43"/>
-      <c r="B47" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="C47" s="66" t="s">
+      <c r="B47" s="66" t="s">
         <v>128</v>
       </c>
+      <c r="C47" s="67" t="s">
+        <v>129</v>
+      </c>
       <c r="D47" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F47" s="26">
         <v>45094.0</v>
@@ -2555,33 +2566,33 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="68"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="71">
+      <c r="B48" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="72">
         <v>45064.0</v>
       </c>
-      <c r="G48" s="71">
+      <c r="G48" s="72">
         <v>45098.0</v>
       </c>
-      <c r="H48" s="72"/>
+      <c r="H48" s="73"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
-      <c r="D49" s="73"/>
-      <c r="E49" s="73"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="75"/>
+      <c r="B50" s="76"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -4375,79 +4386,79 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="B2" s="76" t="s">
-        <v>133</v>
+      <c r="B2" s="77" t="s">
+        <v>134</v>
       </c>
       <c r="C2" s="14"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="B3" s="77" t="s">
-        <v>134</v>
+      <c r="B3" s="78" t="s">
+        <v>135</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="78" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="79" t="s">
+      <c r="B4" s="79" t="s">
         <v>136</v>
       </c>
+      <c r="C4" s="80" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="80" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="81" t="s">
+      <c r="B5" s="81" t="s">
         <v>138</v>
       </c>
+      <c r="C5" s="82" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="80" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="81" t="s">
+      <c r="B6" s="81" t="s">
         <v>140</v>
       </c>
+      <c r="C6" s="82" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="80" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="81" t="s">
+      <c r="B7" s="81" t="s">
         <v>142</v>
       </c>
+      <c r="C7" s="82" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="8" ht="16.5" customHeight="1">
-      <c r="B8" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="81" t="s">
+      <c r="B8" s="83" t="s">
         <v>144</v>
       </c>
+      <c r="C8" s="82" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="80" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" s="81" t="s">
+      <c r="B9" s="81" t="s">
         <v>146</v>
       </c>
+      <c r="C9" s="82" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="80" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="81" t="s">
+      <c r="B10" s="81" t="s">
         <v>148</v>
       </c>
+      <c r="C10" s="82" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="83" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="84" t="s">
+      <c r="B11" s="84" t="s">
         <v>150</v>
+      </c>
+      <c r="C11" s="85" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>

</xml_diff>